<commit_message>
tovabbi 2 tesztfajl hozzaadasa
</commit_message>
<xml_diff>
--- a/tesztkeszlet.xlsx
+++ b/tesztkeszlet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\176246\se-lab-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCB9983-2A82-4216-B4DD-463DBD6D4816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10009A44-4E20-42FA-B432-B849C896F4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22860" yWindow="7935" windowWidth="10605" windowHeight="11385" xr2:uid="{5F7A3981-8BA2-4B63-988E-9E4FEB4849E7}"/>
+    <workbookView xWindow="18195" yWindow="4215" windowWidth="10605" windowHeight="11385" xr2:uid="{5F7A3981-8BA2-4B63-988E-9E4FEB4849E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>Tesztelt követelmény</t>
   </si>
@@ -400,6 +400,27 @@
   </si>
   <si>
     <t>teszt 9</t>
+  </si>
+  <si>
+    <t>teszt10</t>
+  </si>
+  <si>
+    <t>teszt11</t>
+  </si>
+  <si>
+    <t>ugyanaz csak a másik már kiürült ezért a vége fail</t>
+  </si>
+  <si>
+    <t>1 0 1 0</t>
+  </si>
+  <si>
+    <t>succ succ succ fail</t>
+  </si>
+  <si>
+    <t>3 0 1 0</t>
+  </si>
+  <si>
+    <t>succ succ succ succ fail</t>
   </si>
 </sst>
 </file>
@@ -810,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE853FD-7D02-4228-BF52-AB07AD3397FB}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +864,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -860,7 +881,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -877,7 +898,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1287,38 +1308,64 @@
       <c r="B64" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B69" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>62</v>
+      </c>
+      <c r="C71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>